<commit_message>
fixed typo in the word Agrricoltura indicated in issue #96
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-public-services/public-services-subject-matters/public-services-subject-matters.xlsx
+++ b/VocabolariControllati/classifications-for-public-services/public-services-subject-matters/public-services-subject-matters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Dropbox/OntoPiA/SubjectMatterServizi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Dropbox/OntoPiA/GitOntoPiA/daf-ontologie-vocabolari-controllati/VocabolariControllati/classifications-for-public-services/public-services-subject-matters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E927DFC5-D73A-F946-BA7E-611D6FD46191}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336ADDAF-4A64-3845-BAFC-548F6D56EB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{9C134F5D-B371-7146-A492-05301B725373}"/>
   </bookViews>
@@ -20,11 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -167,9 +162,6 @@
     <t>Attività produttive e commercio</t>
   </si>
   <si>
-    <t>Agrricoltura</t>
-  </si>
-  <si>
     <t>Agricoltura - pesca, politiche agricole e alimentari</t>
   </si>
   <si>
@@ -177,6 +169,9 @@
   </si>
   <si>
     <t>Questa materia include tutti quei servizi dell'anagrafe e dello stato civile (per esempio, certificati anagrafici, matrimonio, residenza, domicilio, elezioni, espatrio)</t>
+  </si>
+  <si>
+    <t>Agricoltura</t>
   </si>
 </sst>
 </file>
@@ -569,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB859F7-ADE6-6E42-BAD2-48340E2D9955}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,7 +671,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -796,13 +791,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Revised controlled vocabulary public-services-subject-matters in order to respond to issue #177
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-public-services/public-services-subject-matters/public-services-subject-matters.xlsx
+++ b/VocabolariControllati/classifications-for-public-services/public-services-subject-matters/public-services-subject-matters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Dropbox/OntoPiA/GitOntoPiA/daf-ontologie-vocabolari-controllati/VocabolariControllati/classifications-for-public-services/public-services-subject-matters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336ADDAF-4A64-3845-BAFC-548F6D56EB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19D48BA-2565-0745-998F-E16FD5A56F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{9C134F5D-B371-7146-A492-05301B725373}"/>
   </bookViews>
@@ -78,12 +78,6 @@
     <t>Giustizia e sicurezza pubblica - crimini, protezione civile</t>
   </si>
   <si>
-    <t>Tributi e finanze</t>
-  </si>
-  <si>
-    <t>Tributi e finanze -  dichiarazione redditi, contributi, contravvenzioni</t>
-  </si>
-  <si>
     <t>Cultura e tempo libero</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
     <t>Ambiente - rifiuti, verde urbano, incendi</t>
   </si>
   <si>
-    <t>Attività produttive e commercio - impresa nazionale/estera, notifiche, bancarotta, risorse umane</t>
-  </si>
-  <si>
     <t>Autorizzazioni</t>
   </si>
   <si>
@@ -159,19 +150,28 @@
     <t>Questa materia include tutti quei servizi relativi alla salute degli individui (e.g., prenotazione esami) ma anche tutti i servizi che riguardano l'assistenza e il benessere dei cittadini (e.g., servizi per invalidi, per anziani, per minori). Questo concetto include anche i servizi relativi agli animali</t>
   </si>
   <si>
-    <t>Attività produttive e commercio</t>
-  </si>
-  <si>
-    <t>Agricoltura - pesca, politiche agricole e alimentari</t>
-  </si>
-  <si>
     <t>Questa materia include tutti quei servizi pertinenti al contesto agricolo, della pesca e alimentare</t>
   </si>
   <si>
     <t>Questa materia include tutti quei servizi dell'anagrafe e dello stato civile (per esempio, certificati anagrafici, matrimonio, residenza, domicilio, elezioni, espatrio)</t>
   </si>
   <si>
-    <t>Agricoltura</t>
+    <t>Agricoltura e pesca</t>
+  </si>
+  <si>
+    <t>Tributi, finanze e contravvenzioni</t>
+  </si>
+  <si>
+    <t>Impresa e commercio</t>
+  </si>
+  <si>
+    <t>Impresa e commercio - attività produttive, impresa nazionale/estera, notifiche, bancarotta, risorse umane</t>
+  </si>
+  <si>
+    <t>Agricoltura e pesca - politiche agricole e alimentari</t>
+  </si>
+  <si>
+    <t>Tributi, finanze e contravvenzioni -  dichiarazione redditi, contributi</t>
   </si>
 </sst>
 </file>
@@ -565,7 +565,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,10 +598,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -615,7 +615,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -623,13 +623,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -643,7 +643,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -657,7 +657,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -671,7 +671,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -685,7 +685,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -699,7 +699,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -707,13 +707,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -721,13 +721,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -735,13 +735,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -749,13 +749,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -763,13 +763,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -777,13 +777,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -791,13 +791,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>